<commit_message>
updated example metadata.xlsx and corrections in README.md
</commit_message>
<xml_diff>
--- a/example metadata.xlsx
+++ b/example metadata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stefanhallermann/Library/CloudStorage/Dropbox/tmp/Rinako/in/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43BA674D-79C5-7D46-B50B-E1EDBA5CB1A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16054EB8-C8DE-AD45-A8D6-C9C73A07D50B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="23260" windowHeight="13900" xr2:uid="{86CC86FD-7D8C-8345-B2D7-EF3584566E41}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t>file_name</t>
   </si>
@@ -71,9 +71,6 @@
     <t>fraction_of_max_of_2nd_derivative</t>
   </si>
   <si>
-    <t>filter_cut_off</t>
-  </si>
-  <si>
     <t>window_for_searching_threshold</t>
   </si>
   <si>
@@ -132,6 +129,12 @@
   </si>
   <si>
     <t>rin_series_from_current</t>
+  </si>
+  <si>
+    <t>ap_broadening_series</t>
+  </si>
+  <si>
+    <t>smooth_window</t>
   </si>
 </sst>
 </file>
@@ -203,12 +206,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -523,30 +525,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{990E0E9B-AAB4-D447-83D7-E07861D328B2}">
-  <dimension ref="A1:AC4"/>
+  <dimension ref="A1:AD4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="22.33203125" customWidth="1"/>
-    <col min="6" max="6" width="11.1640625" style="2"/>
-    <col min="8" max="8" width="11.1640625" style="1"/>
-    <col min="9" max="9" width="11" style="2" customWidth="1"/>
-    <col min="12" max="13" width="11.1640625" style="3"/>
-    <col min="14" max="14" width="11.1640625" style="2"/>
-    <col min="17" max="17" width="11.1640625" style="3"/>
-    <col min="18" max="18" width="11.1640625" style="2"/>
-    <col min="21" max="21" width="11.1640625" style="3"/>
-    <col min="22" max="22" width="11.1640625" style="2"/>
-    <col min="25" max="25" width="11.1640625" style="3"/>
-    <col min="26" max="26" width="11.1640625" style="2"/>
-    <col min="29" max="29" width="11.1640625" style="3"/>
+    <col min="7" max="7" width="11.1640625" style="2"/>
+    <col min="9" max="9" width="11.1640625" style="1"/>
+    <col min="10" max="10" width="11" style="2" customWidth="1"/>
+    <col min="13" max="14" width="11.1640625" style="3"/>
+    <col min="15" max="15" width="11.1640625" style="2"/>
+    <col min="18" max="18" width="11.1640625" style="3"/>
+    <col min="19" max="19" width="11.1640625" style="2"/>
+    <col min="22" max="22" width="11.1640625" style="3"/>
+    <col min="23" max="23" width="11.1640625" style="2"/>
+    <col min="26" max="26" width="11.1640625" style="3"/>
+    <col min="27" max="27" width="11.1640625" style="2"/>
+    <col min="30" max="30" width="11.1640625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -562,80 +564,83 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" t="s">
         <v>31</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" t="s">
+        <v>29</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>10</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
+        <v>32</v>
+      </c>
+      <c r="M1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="N1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="O1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="P1" t="s">
         <v>14</v>
       </c>
-      <c r="O1" t="s">
+      <c r="Q1" t="s">
         <v>15</v>
       </c>
-      <c r="P1" t="s">
+      <c r="R1" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="Q1" s="3" t="s">
+      <c r="S1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="T1" t="s">
         <v>18</v>
       </c>
-      <c r="S1" t="s">
+      <c r="U1" t="s">
         <v>19</v>
       </c>
-      <c r="T1" t="s">
+      <c r="V1" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="U1" s="3" t="s">
+      <c r="W1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="V1" s="2" t="s">
+      <c r="X1" t="s">
         <v>22</v>
       </c>
-      <c r="W1" t="s">
+      <c r="Y1" t="s">
         <v>23</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Z1" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="Y1" s="3" t="s">
+      <c r="AA1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="Z1" s="2" t="s">
+      <c r="AB1" t="s">
         <v>26</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AC1" t="s">
         <v>27</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AD1" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="AC1" s="3" t="s">
-        <v>29</v>
-      </c>
     </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -651,80 +656,83 @@
       <c r="E2">
         <v>4</v>
       </c>
-      <c r="F2" s="2">
+      <c r="F2">
+        <v>4</v>
+      </c>
+      <c r="G2" s="2">
         <v>-10000</v>
       </c>
-      <c r="G2" s="4">
+      <c r="H2">
         <v>10000</v>
       </c>
-      <c r="H2" s="1">
+      <c r="I2" s="1">
         <v>-20</v>
       </c>
-      <c r="I2" s="2">
+      <c r="J2" s="2">
         <v>10</v>
       </c>
-      <c r="J2">
-        <v>0.3</v>
-      </c>
       <c r="K2">
-        <v>10000</v>
-      </c>
-      <c r="L2" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="L2">
+        <v>0.1</v>
+      </c>
+      <c r="M2" s="3">
         <v>2E-3</v>
       </c>
-      <c r="M2" s="3">
-        <v>0.01</v>
-      </c>
-      <c r="N2" s="2">
+      <c r="N2" s="3">
+        <v>0.01</v>
+      </c>
+      <c r="O2" s="2">
         <v>1E-3</v>
       </c>
-      <c r="O2">
+      <c r="P2">
         <v>5.0000000000000001E-4</v>
       </c>
-      <c r="P2">
+      <c r="Q2">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="Q2" s="3">
-        <v>0.3</v>
-      </c>
-      <c r="R2" s="2">
-        <v>0.01</v>
-      </c>
-      <c r="S2">
+      <c r="R2" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="S2" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="T2">
         <v>0.09</v>
       </c>
-      <c r="T2">
-        <v>0.3</v>
-      </c>
-      <c r="U2" s="3">
+      <c r="U2">
+        <v>0.3</v>
+      </c>
+      <c r="V2" s="3">
         <v>0.39</v>
       </c>
-      <c r="V2" s="2">
-        <v>0.01</v>
-      </c>
-      <c r="W2">
+      <c r="W2" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="X2">
         <v>0.09</v>
       </c>
-      <c r="X2">
-        <v>0.3</v>
-      </c>
-      <c r="Y2" s="3">
+      <c r="Y2">
+        <v>0.3</v>
+      </c>
+      <c r="Z2" s="3">
         <v>0.39</v>
       </c>
-      <c r="Z2" s="2">
-        <v>0.01</v>
-      </c>
-      <c r="AA2">
+      <c r="AA2" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="AB2">
         <v>0.09</v>
       </c>
-      <c r="AB2">
-        <v>0.3</v>
-      </c>
-      <c r="AC2" s="3">
+      <c r="AC2">
+        <v>0.3</v>
+      </c>
+      <c r="AD2" s="3">
         <v>0.39</v>
       </c>
     </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -738,82 +746,85 @@
         <v>4</v>
       </c>
       <c r="E3">
-        <v>5</v>
-      </c>
-      <c r="F3" s="2">
+        <v>4</v>
+      </c>
+      <c r="F3">
+        <v>4</v>
+      </c>
+      <c r="G3" s="2">
         <v>-10000</v>
       </c>
-      <c r="G3" s="4">
+      <c r="H3">
         <v>10000</v>
       </c>
-      <c r="H3" s="1">
+      <c r="I3" s="1">
         <v>-20</v>
       </c>
-      <c r="I3" s="2">
+      <c r="J3" s="2">
         <v>10</v>
       </c>
-      <c r="J3">
-        <v>0.3</v>
-      </c>
       <c r="K3">
-        <v>10000</v>
-      </c>
-      <c r="L3" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="L3">
+        <v>0.1</v>
+      </c>
+      <c r="M3" s="3">
         <v>2E-3</v>
       </c>
-      <c r="M3" s="3">
-        <v>0.01</v>
-      </c>
-      <c r="N3" s="2">
+      <c r="N3" s="3">
+        <v>0.01</v>
+      </c>
+      <c r="O3" s="2">
         <v>1E-3</v>
       </c>
-      <c r="O3">
+      <c r="P3">
         <v>5.0000000000000001E-4</v>
       </c>
-      <c r="P3">
+      <c r="Q3">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="Q3" s="3">
-        <v>0.3</v>
-      </c>
-      <c r="R3" s="2">
-        <v>0.01</v>
-      </c>
-      <c r="S3">
+      <c r="R3" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="S3" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="T3">
         <v>0.09</v>
       </c>
-      <c r="T3">
-        <v>0.3</v>
-      </c>
-      <c r="U3" s="3">
+      <c r="U3">
+        <v>0.3</v>
+      </c>
+      <c r="V3" s="3">
         <v>0.39</v>
       </c>
-      <c r="V3" s="2">
-        <v>0.01</v>
-      </c>
-      <c r="W3">
+      <c r="W3" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="X3">
         <v>0.09</v>
       </c>
-      <c r="X3">
-        <v>0.3</v>
-      </c>
-      <c r="Y3" s="3">
+      <c r="Y3">
+        <v>0.3</v>
+      </c>
+      <c r="Z3" s="3">
         <v>0.39</v>
       </c>
-      <c r="Z3" s="2">
-        <v>0.01</v>
-      </c>
-      <c r="AA3">
+      <c r="AA3" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="AB3">
         <v>0.09</v>
       </c>
-      <c r="AB3">
-        <v>0.3</v>
-      </c>
-      <c r="AC3" s="3">
+      <c r="AC3">
+        <v>0.3</v>
+      </c>
+      <c r="AD3" s="3">
         <v>0.39</v>
       </c>
     </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -829,76 +840,79 @@
       <c r="E4">
         <v>8</v>
       </c>
-      <c r="F4" s="2">
+      <c r="F4">
+        <v>8</v>
+      </c>
+      <c r="G4" s="2">
         <v>-10000</v>
       </c>
-      <c r="G4" s="4">
+      <c r="H4">
         <v>10000</v>
       </c>
-      <c r="H4" s="1">
+      <c r="I4" s="1">
         <v>-20</v>
       </c>
-      <c r="I4" s="2">
+      <c r="J4" s="2">
         <v>10</v>
       </c>
-      <c r="J4">
-        <v>0.3</v>
-      </c>
       <c r="K4">
-        <v>10000</v>
-      </c>
-      <c r="L4" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="L4">
+        <v>0.1</v>
+      </c>
+      <c r="M4" s="3">
         <v>2E-3</v>
       </c>
-      <c r="M4" s="3">
-        <v>0.01</v>
-      </c>
-      <c r="N4" s="2">
+      <c r="N4" s="3">
+        <v>0.01</v>
+      </c>
+      <c r="O4" s="2">
         <v>1E-3</v>
       </c>
-      <c r="O4">
+      <c r="P4">
         <v>5.0000000000000001E-4</v>
       </c>
-      <c r="P4">
+      <c r="Q4">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="Q4" s="3">
-        <v>0.3</v>
-      </c>
-      <c r="R4" s="2">
-        <v>0.01</v>
-      </c>
-      <c r="S4">
+      <c r="R4" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="S4" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="T4">
         <v>0.09</v>
       </c>
-      <c r="T4">
-        <v>0.3</v>
-      </c>
-      <c r="U4" s="3">
+      <c r="U4">
+        <v>0.3</v>
+      </c>
+      <c r="V4" s="3">
         <v>0.39</v>
       </c>
-      <c r="V4" s="2">
-        <v>0.01</v>
-      </c>
-      <c r="W4">
+      <c r="W4" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="X4">
         <v>0.09</v>
       </c>
-      <c r="X4">
-        <v>0.3</v>
-      </c>
-      <c r="Y4" s="3">
+      <c r="Y4">
+        <v>0.3</v>
+      </c>
+      <c r="Z4" s="3">
         <v>0.39</v>
       </c>
-      <c r="Z4" s="2">
-        <v>0.01</v>
-      </c>
-      <c r="AA4">
+      <c r="AA4" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="AB4">
         <v>0.09</v>
       </c>
-      <c r="AB4">
-        <v>0.3</v>
-      </c>
-      <c r="AC4" s="3">
+      <c r="AC4">
+        <v>0.3</v>
+      </c>
+      <c r="AD4" s="3">
         <v>0.39</v>
       </c>
     </row>

</xml_diff>